<commit_message>
Agregando la funcionalidad del Rol y asignación de menus al rol
</commit_message>
<xml_diff>
--- a/database/seeders/Catalogos/RolMenu.xlsx
+++ b/database/seeders/Catalogos/RolMenu.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>Catálogos</t>
   </si>
@@ -431,7 +431,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,10 +493,13 @@
         <v>2</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>21</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -513,10 +516,13 @@
         <v>4</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>21</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>